<commit_message>
docs: permissões das colunas is_email_verificado, is_telefone_verificado e status (auth)
</commit_message>
<xml_diff>
--- a/banco-de-dados/docs/4-tabelas-permissoes/tabelas-permissoes.xlsx
+++ b/banco-de-dados/docs/4-tabelas-permissoes/tabelas-permissoes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gsouza\Desktop\repositorios\TG_Fatec\banco-de-dados\docs\4-tabelas-permissoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsouza\Desktop\repositorios\meus-projetos\TG_Fatec\banco-de-dados\docs\4-tabelas-permissoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75B9E3E-1773-49A4-86AA-564BAA360B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AF427B-18C4-4291-B2CB-E2F10AF7DDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-storage" sheetId="6" r:id="rId1"/>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="121">
   <si>
     <t>INSERT</t>
   </si>
@@ -145,42 +145,12 @@
     <t xml:space="preserve">    deleted_at</t>
   </si>
   <si>
-    <t xml:space="preserve">    last_access</t>
-  </si>
-  <si>
     <t xml:space="preserve">    is_deleted</t>
   </si>
   <si>
-    <t xml:space="preserve">    cpf</t>
-  </si>
-  <si>
     <t xml:space="preserve">    nome</t>
   </si>
   <si>
-    <t xml:space="preserve">    sobrenome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    nome_social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    sobrenome_social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    sexo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    data_nascimento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    telefone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    senha</t>
-  </si>
-  <si>
     <t xml:space="preserve">    s_storage_t_tb_arquivo_c_foto</t>
   </si>
   <si>
@@ -449,6 +419,48 @@
   </si>
   <si>
     <t>cor_led</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>last_access</t>
+  </si>
+  <si>
+    <t>cpf</t>
+  </si>
+  <si>
+    <t>sobrenome</t>
+  </si>
+  <si>
+    <t>nome_social</t>
+  </si>
+  <si>
+    <t>sobrenome_social</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>data_nascimento</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>s_storage_t_tb_arquivo_c_foto</t>
+  </si>
+  <si>
+    <t>is_email_verificado</t>
+  </si>
+  <si>
+    <t>is_telefone_verificado</t>
   </si>
 </sst>
 </file>
@@ -502,7 +514,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -968,21 +980,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -1164,11 +1161,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1266,46 +1298,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1335,9 +1367,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1353,101 +1448,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1837,62 +1860,62 @@
   <sheetData>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="79"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="61"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="82"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="67"/>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="77"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -1939,21 +1962,21 @@
         <v>5</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="62"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="22"/>
       <c r="H8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="62"/>
+      <c r="J8" s="59"/>
       <c r="K8" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="M8" s="14"/>
-      <c r="N8" s="62"/>
+      <c r="N8" s="59"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -1962,11 +1985,11 @@
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="63"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="63"/>
+      <c r="J9" s="60"/>
       <c r="K9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1997,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="63"/>
+      <c r="N9" s="60"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1983,11 +2006,11 @@
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="63"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="63"/>
+      <c r="J10" s="60"/>
       <c r="K10" s="4" t="s">
         <v>6</v>
       </c>
@@ -1997,7 +2020,7 @@
       <c r="M10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="63"/>
+      <c r="N10" s="60"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -2006,11 +2029,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="63"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="4"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
-      <c r="J11" s="63"/>
+      <c r="J11" s="60"/>
       <c r="K11" s="4" t="s">
         <v>7</v>
       </c>
@@ -2020,24 +2043,24 @@
       <c r="M11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="63"/>
+      <c r="N11" s="60"/>
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="63"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="4"/>
       <c r="H12" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="27"/>
-      <c r="J12" s="63"/>
+      <c r="J12" s="60"/>
       <c r="K12" s="4" t="s">
         <v>6</v>
       </c>
@@ -2047,24 +2070,24 @@
       <c r="M12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="63"/>
+      <c r="N12" s="60"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="63"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="4"/>
       <c r="H13" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="27"/>
-      <c r="J13" s="63"/>
+      <c r="J13" s="60"/>
       <c r="K13" s="4" t="s">
         <v>5</v>
       </c>
@@ -2074,26 +2097,26 @@
       <c r="M13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="63"/>
+      <c r="N13" s="60"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="63"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="4"/>
       <c r="H14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="63"/>
+      <c r="J14" s="60"/>
       <c r="K14" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L14" s="27" t="s">
         <v>5</v>
@@ -2101,26 +2124,26 @@
       <c r="M14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N14" s="63"/>
+      <c r="N14" s="60"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="27"/>
-      <c r="F15" s="63"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="4"/>
       <c r="H15" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="27"/>
-      <c r="J15" s="63"/>
+      <c r="J15" s="60"/>
       <c r="K15" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L15" s="27" t="s">
         <v>5</v>
@@ -2128,26 +2151,26 @@
       <c r="M15" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="63"/>
+      <c r="N15" s="60"/>
     </row>
     <row r="16" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="64"/>
+      <c r="F16" s="61"/>
       <c r="G16" s="7"/>
       <c r="H16" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="19"/>
-      <c r="J16" s="64"/>
+      <c r="J16" s="61"/>
       <c r="K16" s="7" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="L16" s="19" t="s">
         <v>5</v>
@@ -2155,52 +2178,52 @@
       <c r="M16" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="64"/>
+      <c r="N16" s="61"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="67"/>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="68"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="70"/>
+    </row>
+    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="76"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="77"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="79"/>
-    </row>
-    <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="80"/>
-      <c r="G22" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="67"/>
+      <c r="C22" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="77"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="71"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="10" t="s">
         <v>0</v>
       </c>
@@ -2231,21 +2254,21 @@
         <v>4</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="14"/>
-      <c r="F24" s="62"/>
+      <c r="F24" s="59"/>
       <c r="G24" s="15" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H24" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="23"/>
-      <c r="J24" s="72"/>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
@@ -2256,7 +2279,7 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="63"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="4" t="s">
         <v>6</v>
       </c>
@@ -2264,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="I25" s="25"/>
-      <c r="J25" s="73"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
@@ -2275,7 +2298,7 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="63"/>
+      <c r="F26" s="60"/>
       <c r="G26" s="4" t="s">
         <v>7</v>
       </c>
@@ -2285,18 +2308,18 @@
       <c r="I26" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="73"/>
+      <c r="J26" s="63"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="63"/>
+      <c r="F27" s="60"/>
       <c r="G27" s="26" t="s">
         <v>5</v>
       </c>
@@ -2304,18 +2327,18 @@
         <v>5</v>
       </c>
       <c r="I27" s="27"/>
-      <c r="J27" s="73"/>
+      <c r="J27" s="63"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="63"/>
+      <c r="F28" s="60"/>
       <c r="G28" s="26" t="s">
         <v>7</v>
       </c>
@@ -2325,18 +2348,18 @@
       <c r="I28" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="63"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="63"/>
+      <c r="F29" s="60"/>
       <c r="G29" s="26" t="s">
         <v>6</v>
       </c>
@@ -2346,18 +2369,18 @@
       <c r="I29" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="73"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="63"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="26" t="s">
         <v>5</v>
       </c>
@@ -2365,18 +2388,18 @@
         <v>5</v>
       </c>
       <c r="I30" s="27"/>
-      <c r="J30" s="73"/>
+      <c r="J30" s="63"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="63"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="26" t="s">
         <v>5</v>
       </c>
@@ -2384,35 +2407,35 @@
         <v>5</v>
       </c>
       <c r="I31" s="27"/>
-      <c r="J31" s="73"/>
+      <c r="J31" s="63"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="63"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
-      <c r="J32" s="73"/>
+      <c r="J32" s="63"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="63"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="26" t="s">
         <v>5</v>
       </c>
@@ -2420,18 +2443,18 @@
         <v>5</v>
       </c>
       <c r="I33" s="27"/>
-      <c r="J33" s="73"/>
+      <c r="J33" s="63"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C34" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="63"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="30" t="s">
         <v>5</v>
       </c>
@@ -2439,18 +2462,18 @@
         <v>5</v>
       </c>
       <c r="I34" s="31"/>
-      <c r="J34" s="73"/>
+      <c r="J34" s="63"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
-      <c r="F35" s="64"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="18" t="s">
         <v>5</v>
       </c>
@@ -2458,7 +2481,7 @@
         <v>5</v>
       </c>
       <c r="I35" s="19"/>
-      <c r="J35" s="74"/>
+      <c r="J35" s="64"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2509,12 +2532,6 @@
     <row r="245" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F24:F35"/>
-    <mergeCell ref="J24:J35"/>
-    <mergeCell ref="B20:J21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:J22"/>
     <mergeCell ref="B4:N5"/>
     <mergeCell ref="N8:N16"/>
     <mergeCell ref="K6:N6"/>
@@ -2523,6 +2540,12 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="F8:F16"/>
+    <mergeCell ref="F24:F35"/>
+    <mergeCell ref="J24:J35"/>
+    <mergeCell ref="B20:J21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:J22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2533,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CFD5EC-BE05-41AD-8BD3-9CD7478A622B}">
   <dimension ref="B3:J245"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,48 +2567,48 @@
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="76"/>
+      <c r="B4" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="77"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -2616,38 +2639,38 @@
         <v>4</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="81"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="23"/>
-      <c r="J8" s="84"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="82"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="24"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
-      <c r="J9" s="85"/>
+      <c r="J9" s="63"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
@@ -2656,58 +2679,60 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="82"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="85"/>
+      <c r="J10" s="63"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="82"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="26"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="85"/>
+      <c r="J11" s="63"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="82"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="26"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="85"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="82"/>
+      <c r="E13" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="60"/>
       <c r="G13" s="26"/>
       <c r="H13" s="27" t="s">
         <v>5</v>
@@ -2715,11 +2740,11 @@
       <c r="I13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="85"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>5</v>
@@ -2728,24 +2753,24 @@
         <v>5</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="82"/>
+      <c r="F14" s="60"/>
       <c r="G14" s="26"/>
       <c r="H14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="27"/>
-      <c r="J14" s="85"/>
+      <c r="J14" s="63"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27"/>
-      <c r="F15" s="82"/>
+      <c r="F15" s="60"/>
       <c r="G15" s="26"/>
       <c r="H15" s="27" t="s">
         <v>5</v>
@@ -2753,18 +2778,18 @@
       <c r="I15" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="85"/>
+      <c r="J15" s="63"/>
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="82"/>
+      <c r="F16" s="60"/>
       <c r="G16" s="26"/>
       <c r="H16" s="27" t="s">
         <v>5</v>
@@ -2772,18 +2797,18 @@
       <c r="I16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="85"/>
+      <c r="J16" s="63"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
-      <c r="F17" s="82"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="26"/>
       <c r="H17" s="27" t="s">
         <v>5</v>
@@ -2791,18 +2816,18 @@
       <c r="I17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="85"/>
+      <c r="J17" s="63"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="27"/>
-      <c r="F18" s="82"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="26"/>
       <c r="H18" s="27" t="s">
         <v>5</v>
@@ -2810,35 +2835,35 @@
       <c r="I18" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="85"/>
+      <c r="J18" s="63"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>113</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27"/>
-      <c r="F19" s="82"/>
+      <c r="F19" s="60"/>
       <c r="G19" s="26"/>
       <c r="H19" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="27"/>
-      <c r="J19" s="85"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="82"/>
+      <c r="F20" s="60"/>
       <c r="G20" s="26"/>
       <c r="H20" s="27" t="s">
         <v>5</v>
@@ -2846,11 +2871,11 @@
       <c r="I20" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="85"/>
+      <c r="J20" s="63"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>5</v>
@@ -2859,26 +2884,28 @@
         <v>5</v>
       </c>
       <c r="E21" s="27"/>
-      <c r="F21" s="82"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="26"/>
       <c r="H21" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I21" s="27"/>
-      <c r="J21" s="85"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>25</v>
+      <c r="B22" s="90" t="s">
+        <v>119</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="82"/>
+      <c r="E22" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="60"/>
       <c r="G22" s="26"/>
       <c r="H22" s="27" t="s">
         <v>5</v>
@@ -2886,11 +2913,11 @@
       <c r="I22" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="85"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>5</v>
@@ -2898,10 +2925,8 @@
       <c r="D23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="82"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="26"/>
       <c r="H23" s="27" t="s">
         <v>5</v>
@@ -2909,200 +2934,208 @@
       <c r="I23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="85"/>
-    </row>
-    <row r="24" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="83"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" s="86"/>
-    </row>
-    <row r="26" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="76"/>
-    </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="79"/>
-    </row>
+      <c r="J23" s="63"/>
+    </row>
+    <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="60"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="63"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="60"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="63"/>
+    </row>
+    <row r="26" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="61"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" s="64"/>
+    </row>
+    <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="65" t="s">
-        <v>69</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
       <c r="H30" s="66"/>
       <c r="I30" s="66"/>
       <c r="J30" s="67"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="71"/>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="70"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="77"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="89"/>
+      <c r="C33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="72"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="73"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="I34" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="73"/>
+      <c r="C34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="23"/>
+      <c r="J34" s="62"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I35" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="73"/>
+        <v>13</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="63"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="73"/>
+        <v>20</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="63"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="63"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="26"/>
       <c r="H37" s="27" t="s">
         <v>5</v>
@@ -3110,18 +3143,18 @@
       <c r="I37" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J37" s="73"/>
+      <c r="J37" s="63"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
-      <c r="F38" s="63"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="26"/>
       <c r="H38" s="27" t="s">
         <v>5</v>
@@ -3129,18 +3162,18 @@
       <c r="I38" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="73"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
-      <c r="F39" s="63"/>
+      <c r="F39" s="60"/>
       <c r="G39" s="26"/>
       <c r="H39" s="27" t="s">
         <v>5</v>
@@ -3148,26 +3181,64 @@
       <c r="I39" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="73"/>
-    </row>
-    <row r="40" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" s="74"/>
+      <c r="J39" s="63"/>
+    </row>
+    <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="63"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="63"/>
+    </row>
+    <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="64"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3215,18 +3286,18 @@
     <row r="245" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="F32:F40"/>
-    <mergeCell ref="J32:J40"/>
-    <mergeCell ref="F8:F24"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="J8:J26"/>
+    <mergeCell ref="F8:F26"/>
     <mergeCell ref="B4:J5"/>
-    <mergeCell ref="J8:J24"/>
-    <mergeCell ref="B28:J29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="B30:J31"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="G6:J6"/>
+    <mergeCell ref="J34:J42"/>
+    <mergeCell ref="F34:F42"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="C32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3248,48 +3319,48 @@
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="76"/>
+      <c r="B4" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="77"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="79"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="70"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -3324,13 +3395,13 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="62"/>
+      <c r="F8" s="59"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="23"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -3341,7 +3412,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="63"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="24"/>
       <c r="H9" s="25" t="s">
         <v>5</v>
@@ -3349,18 +3420,18 @@
       <c r="I9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="73"/>
+      <c r="J9" s="63"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="63"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="24"/>
       <c r="H10" s="25" t="s">
         <v>5</v>
@@ -3368,18 +3439,18 @@
       <c r="I10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="63"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C11" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
-      <c r="F11" s="63"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="26"/>
       <c r="H11" s="27" t="s">
         <v>5</v>
@@ -3387,18 +3458,18 @@
       <c r="I11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="73"/>
+      <c r="J11" s="63"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="64"/>
+      <c r="F12" s="61"/>
       <c r="G12" s="18"/>
       <c r="H12" s="19" t="s">
         <v>5</v>
@@ -3406,53 +3477,53 @@
       <c r="I12" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="74"/>
+      <c r="J12" s="64"/>
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="76"/>
+      <c r="B16" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="67"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="79"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="70"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="67"/>
+      <c r="B18" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="77"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="10" t="s">
         <v>0</v>
       </c>
@@ -3487,13 +3558,13 @@
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="62"/>
+      <c r="F20" s="59"/>
       <c r="G20" s="22"/>
       <c r="H20" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="23"/>
-      <c r="J20" s="72"/>
+      <c r="J20" s="62"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
@@ -3504,7 +3575,7 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="63"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="24"/>
       <c r="H21" s="25" t="s">
         <v>5</v>
@@ -3512,18 +3583,18 @@
       <c r="I21" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="73"/>
+      <c r="J21" s="63"/>
     </row>
     <row r="22" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="63"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="24"/>
       <c r="H22" s="25" t="s">
         <v>5</v>
@@ -3531,18 +3602,18 @@
       <c r="I22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="73"/>
+      <c r="J22" s="63"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="63"/>
+      <c r="F23" s="60"/>
       <c r="G23" s="26"/>
       <c r="H23" s="27" t="s">
         <v>5</v>
@@ -3550,18 +3621,18 @@
       <c r="I23" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="73"/>
+      <c r="J23" s="63"/>
     </row>
     <row r="24" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="63"/>
+      <c r="F24" s="60"/>
       <c r="G24" s="24"/>
       <c r="H24" s="25" t="s">
         <v>5</v>
@@ -3569,18 +3640,18 @@
       <c r="I24" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="73"/>
+      <c r="J24" s="63"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="63"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="26"/>
       <c r="H25" s="27" t="s">
         <v>5</v>
@@ -3588,18 +3659,18 @@
       <c r="I25" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="73"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="64"/>
+      <c r="F26" s="61"/>
       <c r="G26" s="18"/>
       <c r="H26" s="19" t="s">
         <v>5</v>
@@ -3607,53 +3678,53 @@
       <c r="I26" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="74"/>
+      <c r="J26" s="64"/>
     </row>
     <row r="27" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="76"/>
+      <c r="B30" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="67"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="79"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="70"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="67"/>
+      <c r="B32" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="76"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="77"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="71"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="10" t="s">
         <v>0</v>
       </c>
@@ -3688,13 +3759,13 @@
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
-      <c r="F34" s="62"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="22"/>
       <c r="H34" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I34" s="23"/>
-      <c r="J34" s="72"/>
+      <c r="J34" s="62"/>
     </row>
     <row r="35" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
@@ -3705,7 +3776,7 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="63"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="24"/>
       <c r="H35" s="25" t="s">
         <v>5</v>
@@ -3713,18 +3784,18 @@
       <c r="I35" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="73"/>
+      <c r="J35" s="63"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="63"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="24"/>
       <c r="H36" s="25" t="s">
         <v>5</v>
@@ -3732,18 +3803,18 @@
       <c r="I36" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J36" s="73"/>
+      <c r="J36" s="63"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="63"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="26"/>
       <c r="H37" s="27" t="s">
         <v>5</v>
@@ -3751,18 +3822,18 @@
       <c r="I37" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J37" s="73"/>
+      <c r="J37" s="63"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="63"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="24"/>
       <c r="H38" s="25" t="s">
         <v>5</v>
@@ -3770,18 +3841,18 @@
       <c r="I38" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="73"/>
+      <c r="J38" s="63"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="27"/>
       <c r="E39" s="27"/>
-      <c r="F39" s="63"/>
+      <c r="F39" s="60"/>
       <c r="G39" s="26"/>
       <c r="H39" s="27" t="s">
         <v>5</v>
@@ -3789,18 +3860,18 @@
       <c r="I39" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="73"/>
+      <c r="J39" s="63"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="63"/>
+      <c r="F40" s="60"/>
       <c r="G40" s="24"/>
       <c r="H40" s="25" t="s">
         <v>5</v>
@@ -3808,18 +3879,18 @@
       <c r="I40" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="73"/>
+      <c r="J40" s="63"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="63"/>
+      <c r="F41" s="60"/>
       <c r="G41" s="24"/>
       <c r="H41" s="25" t="s">
         <v>5</v>
@@ -3827,18 +3898,18 @@
       <c r="I41" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J41" s="73"/>
+      <c r="J41" s="63"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
-      <c r="F42" s="63"/>
+      <c r="F42" s="60"/>
       <c r="G42" s="26"/>
       <c r="H42" s="27" t="s">
         <v>5</v>
@@ -3846,18 +3917,18 @@
       <c r="I42" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="73"/>
+      <c r="J42" s="63"/>
     </row>
     <row r="43" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="64"/>
+      <c r="F43" s="61"/>
       <c r="G43" s="28"/>
       <c r="H43" s="29" t="s">
         <v>5</v>
@@ -3865,7 +3936,7 @@
       <c r="I43" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="74"/>
+      <c r="J43" s="64"/>
     </row>
     <row r="44" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3913,6 +3984,14 @@
     <row r="245" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B16:J17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B4:J5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="J8:J12"/>
+    <mergeCell ref="F8:F12"/>
     <mergeCell ref="F34:F43"/>
     <mergeCell ref="J34:J43"/>
     <mergeCell ref="C18:F18"/>
@@ -3923,14 +4002,6 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:F32"/>
     <mergeCell ref="G32:J32"/>
-    <mergeCell ref="B16:J17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B4:J5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="F8:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3941,8 +4012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF00015-3388-4FE7-BF36-AB810A7ADABD}">
   <dimension ref="B3:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,48 +4023,48 @@
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="61"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="67"/>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -4026,24 +4097,24 @@
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
       <c r="E8" s="54"/>
-      <c r="F8" s="72"/>
+      <c r="F8" s="62"/>
       <c r="G8" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="52"/>
-      <c r="J8" s="72"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="25"/>
       <c r="E9" s="48"/>
-      <c r="F9" s="73"/>
+      <c r="F9" s="63"/>
       <c r="G9" s="24" t="s">
         <v>6</v>
       </c>
@@ -4051,16 +4122,16 @@
         <v>5</v>
       </c>
       <c r="I9" s="25"/>
-      <c r="J9" s="73"/>
+      <c r="J9" s="63"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
       <c r="E10" s="48"/>
-      <c r="F10" s="73"/>
+      <c r="F10" s="63"/>
       <c r="G10" s="24" t="s">
         <v>6</v>
       </c>
@@ -4070,16 +4141,16 @@
       <c r="I10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="73"/>
+      <c r="J10" s="63"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="27"/>
       <c r="E11" s="48"/>
-      <c r="F11" s="73"/>
+      <c r="F11" s="63"/>
       <c r="G11" s="24" t="s">
         <v>7</v>
       </c>
@@ -4089,18 +4160,18 @@
       <c r="I11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="73"/>
+      <c r="J11" s="63"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="48"/>
-      <c r="F12" s="73"/>
+      <c r="F12" s="63"/>
       <c r="G12" s="24" t="s">
         <v>6</v>
       </c>
@@ -4110,18 +4181,18 @@
       <c r="I12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="73"/>
+      <c r="J12" s="63"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="48"/>
-      <c r="F13" s="73"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="24" t="s">
         <v>5</v>
       </c>
@@ -4131,18 +4202,18 @@
       <c r="I13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="73"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="55"/>
-      <c r="F14" s="74"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="28" t="s">
         <v>5</v>
       </c>
@@ -4152,38 +4223,38 @@
       <c r="I14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="74"/>
+      <c r="J14" s="64"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="58"/>
+      <c r="B18" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="79"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="61"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="82"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="67"/>
+      <c r="B20" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="77"/>
     </row>
     <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="10" t="s">
         <v>0</v>
       </c>
@@ -4202,17 +4273,17 @@
         <v>4</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="23"/>
-      <c r="F22" s="91"/>
+      <c r="F22" s="56"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>6</v>
@@ -4221,11 +4292,11 @@
         <v>5</v>
       </c>
       <c r="E23" s="25"/>
-      <c r="F23" s="92"/>
+      <c r="F23" s="57"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>5</v>
@@ -4234,11 +4305,11 @@
         <v>5</v>
       </c>
       <c r="E24" s="25"/>
-      <c r="F24" s="92"/>
+      <c r="F24" s="57"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>5</v>
@@ -4247,11 +4318,11 @@
         <v>5</v>
       </c>
       <c r="E25" s="27"/>
-      <c r="F25" s="92"/>
+      <c r="F25" s="57"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>6</v>
@@ -4260,11 +4331,11 @@
         <v>5</v>
       </c>
       <c r="E26" s="27"/>
-      <c r="F26" s="92"/>
+      <c r="F26" s="57"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>5</v>
@@ -4273,11 +4344,11 @@
         <v>5</v>
       </c>
       <c r="E27" s="32"/>
-      <c r="F27" s="92"/>
+      <c r="F27" s="57"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C28" s="36" t="s">
         <v>5</v>
@@ -4286,11 +4357,11 @@
         <v>5</v>
       </c>
       <c r="E28" s="33"/>
-      <c r="F28" s="92"/>
+      <c r="F28" s="57"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>5</v>
@@ -4299,11 +4370,11 @@
         <v>5</v>
       </c>
       <c r="E29" s="33"/>
-      <c r="F29" s="92"/>
+      <c r="F29" s="57"/>
     </row>
     <row r="30" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="39" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C30" s="37" t="s">
         <v>5</v>
@@ -4312,49 +4383,49 @@
         <v>5</v>
       </c>
       <c r="E30" s="38"/>
-      <c r="F30" s="93"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
-      <c r="J34" s="58"/>
+      <c r="B34" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="79"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="59"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="61"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="82"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="66"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="67"/>
+        <v>61</v>
+      </c>
+      <c r="C36" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="77"/>
     </row>
     <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
@@ -4388,45 +4459,45 @@
         <v>4</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D38" s="23"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="72"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="22"/>
       <c r="H38" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I38" s="23"/>
-      <c r="J38" s="72"/>
+      <c r="J38" s="62"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
-      <c r="F39" s="73"/>
+      <c r="F39" s="63"/>
       <c r="G39" s="24"/>
       <c r="H39" s="25"/>
       <c r="I39" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="73"/>
+      <c r="J39" s="63"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C40" s="24" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
-      <c r="F40" s="73"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="24"/>
       <c r="H40" s="25" t="s">
         <v>5</v>
@@ -4434,83 +4505,83 @@
       <c r="I40" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="73"/>
+      <c r="J40" s="63"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
-      <c r="F41" s="73"/>
+      <c r="F41" s="63"/>
       <c r="G41" s="24"/>
       <c r="H41" s="27" t="s">
         <v>5</v>
       </c>
       <c r="I41" s="27"/>
-      <c r="J41" s="73"/>
+      <c r="J41" s="63"/>
     </row>
     <row r="42" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C42" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="74"/>
+      <c r="F42" s="64"/>
       <c r="G42" s="28"/>
       <c r="H42" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I42" s="19"/>
-      <c r="J42" s="74"/>
+      <c r="J42" s="64"/>
     </row>
     <row r="45" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="58"/>
+      <c r="B46" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="78"/>
+      <c r="D46" s="78"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="78"/>
+      <c r="J46" s="79"/>
     </row>
     <row r="47" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="59"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="61"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="81"/>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="82"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48" s="66"/>
-      <c r="E48" s="66"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="H48" s="66"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="67"/>
+        <v>61</v>
+      </c>
+      <c r="C48" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="77"/>
+      <c r="G48" s="71" t="s">
+        <v>81</v>
+      </c>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+      <c r="J48" s="77"/>
     </row>
     <row r="49" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="6"/>
@@ -4546,24 +4617,24 @@
       <c r="C50" s="49"/>
       <c r="D50" s="23"/>
       <c r="E50" s="23"/>
-      <c r="F50" s="87"/>
+      <c r="F50" s="84"/>
       <c r="G50" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H50" s="23" t="s">
         <v>5</v>
       </c>
       <c r="I50" s="23"/>
-      <c r="J50" s="87"/>
+      <c r="J50" s="84"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C51" s="50"/>
       <c r="D51" s="25"/>
       <c r="E51" s="25"/>
-      <c r="F51" s="88"/>
+      <c r="F51" s="85"/>
       <c r="G51" s="24" t="s">
         <v>6</v>
       </c>
@@ -4571,16 +4642,16 @@
         <v>5</v>
       </c>
       <c r="I51" s="25"/>
-      <c r="J51" s="88"/>
+      <c r="J51" s="85"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C52" s="50"/>
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
-      <c r="F52" s="88"/>
+      <c r="F52" s="85"/>
       <c r="G52" s="24" t="s">
         <v>6</v>
       </c>
@@ -4590,16 +4661,16 @@
       <c r="I52" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J52" s="88"/>
+      <c r="J52" s="85"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="13" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="32"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="88"/>
+      <c r="F53" s="85"/>
       <c r="G53" s="24" t="s">
         <v>7</v>
       </c>
@@ -4609,18 +4680,18 @@
       <c r="I53" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="88"/>
+      <c r="J53" s="85"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="34" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C54" s="50"/>
       <c r="D54" s="33" t="s">
         <v>5</v>
       </c>
       <c r="E54" s="33"/>
-      <c r="F54" s="88"/>
+      <c r="F54" s="85"/>
       <c r="G54" s="24" t="s">
         <v>6</v>
       </c>
@@ -4630,18 +4701,18 @@
       <c r="I54" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="J54" s="88"/>
+      <c r="J54" s="85"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="34" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C55" s="50"/>
       <c r="D55" s="33" t="s">
         <v>5</v>
       </c>
       <c r="E55" s="33"/>
-      <c r="F55" s="88"/>
+      <c r="F55" s="85"/>
       <c r="G55" s="24" t="s">
         <v>5</v>
       </c>
@@ -4651,18 +4722,18 @@
       <c r="I55" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="J55" s="88"/>
+      <c r="J55" s="85"/>
     </row>
     <row r="56" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="39" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C56" s="51"/>
       <c r="D56" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E56" s="38"/>
-      <c r="F56" s="90"/>
+      <c r="F56" s="86"/>
       <c r="G56" s="28" t="s">
         <v>5</v>
       </c>
@@ -4672,49 +4743,49 @@
       <c r="I56" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="J56" s="90"/>
+      <c r="J56" s="86"/>
     </row>
     <row r="59" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="58"/>
+      <c r="B60" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="78"/>
+      <c r="D60" s="78"/>
+      <c r="E60" s="78"/>
+      <c r="F60" s="78"/>
+      <c r="G60" s="78"/>
+      <c r="H60" s="78"/>
+      <c r="I60" s="78"/>
+      <c r="J60" s="79"/>
     </row>
     <row r="61" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="59"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="61"/>
+      <c r="B61" s="80"/>
+      <c r="C61" s="81"/>
+      <c r="D61" s="81"/>
+      <c r="E61" s="81"/>
+      <c r="F61" s="81"/>
+      <c r="G61" s="81"/>
+      <c r="H61" s="81"/>
+      <c r="I61" s="81"/>
+      <c r="J61" s="82"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="D62" s="66"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="H62" s="66"/>
-      <c r="I62" s="66"/>
-      <c r="J62" s="67"/>
+        <v>61</v>
+      </c>
+      <c r="C62" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="77"/>
+      <c r="G62" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="77"/>
     </row>
     <row r="63" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="6"/>
@@ -4752,39 +4823,39 @@
       </c>
       <c r="D64" s="23"/>
       <c r="E64" s="23"/>
-      <c r="F64" s="87"/>
+      <c r="F64" s="84"/>
       <c r="G64" s="20"/>
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
-      <c r="J64" s="87"/>
+      <c r="J64" s="84"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" s="43" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C65" s="40" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="25"/>
       <c r="E65" s="25"/>
-      <c r="F65" s="88"/>
+      <c r="F65" s="85"/>
       <c r="G65" s="40"/>
       <c r="H65" s="25"/>
       <c r="I65" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J65" s="88"/>
+      <c r="J65" s="85"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="43" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
-      <c r="F66" s="88"/>
+      <c r="F66" s="85"/>
       <c r="G66" s="40"/>
       <c r="H66" s="25" t="s">
         <v>5</v>
@@ -4792,18 +4863,18 @@
       <c r="I66" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J66" s="88"/>
+      <c r="J66" s="85"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="43" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C67" s="40" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="27"/>
       <c r="E67" s="27"/>
-      <c r="F67" s="88"/>
+      <c r="F67" s="85"/>
       <c r="G67" s="40"/>
       <c r="H67" s="27" t="s">
         <v>5</v>
@@ -4811,18 +4882,18 @@
       <c r="I67" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J67" s="88"/>
+      <c r="J67" s="85"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="43" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C68" s="40" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="27"/>
       <c r="E68" s="27"/>
-      <c r="F68" s="88"/>
+      <c r="F68" s="85"/>
       <c r="G68" s="40"/>
       <c r="H68" s="27" t="s">
         <v>5</v>
@@ -4830,18 +4901,18 @@
       <c r="I68" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J68" s="88"/>
+      <c r="J68" s="85"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="43" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C69" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="32"/>
       <c r="E69" s="32"/>
-      <c r="F69" s="88"/>
+      <c r="F69" s="85"/>
       <c r="G69" s="41"/>
       <c r="H69" s="32" t="s">
         <v>5</v>
@@ -4849,18 +4920,18 @@
       <c r="I69" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="J69" s="88"/>
+      <c r="J69" s="85"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="43" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="33"/>
       <c r="E70" s="33"/>
-      <c r="F70" s="88"/>
+      <c r="F70" s="85"/>
       <c r="G70" s="42"/>
       <c r="H70" s="33" t="s">
         <v>5</v>
@@ -4868,18 +4939,18 @@
       <c r="I70" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="J70" s="88"/>
+      <c r="J70" s="85"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" s="46" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C71" s="44" t="s">
         <v>7</v>
       </c>
       <c r="D71" s="45"/>
       <c r="E71" s="45"/>
-      <c r="F71" s="88"/>
+      <c r="F71" s="85"/>
       <c r="G71" s="44"/>
       <c r="H71" s="45" t="s">
         <v>5</v>
@@ -4887,18 +4958,18 @@
       <c r="I71" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="J71" s="88"/>
+      <c r="J71" s="85"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" s="43" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C72" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="27"/>
       <c r="E72" s="27"/>
-      <c r="F72" s="88"/>
+      <c r="F72" s="85"/>
       <c r="G72" s="26"/>
       <c r="H72" s="27" t="s">
         <v>5</v>
@@ -4906,18 +4977,18 @@
       <c r="I72" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J72" s="88"/>
+      <c r="J72" s="85"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="43" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="27"/>
       <c r="E73" s="27"/>
-      <c r="F73" s="88"/>
+      <c r="F73" s="85"/>
       <c r="G73" s="26"/>
       <c r="H73" s="27" t="s">
         <v>5</v>
@@ -4925,18 +4996,18 @@
       <c r="I73" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J73" s="88"/>
+      <c r="J73" s="85"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" s="43" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="27"/>
       <c r="E74" s="27"/>
-      <c r="F74" s="88"/>
+      <c r="F74" s="85"/>
       <c r="G74" s="26"/>
       <c r="H74" s="27" t="s">
         <v>5</v>
@@ -4944,18 +5015,18 @@
       <c r="I74" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J74" s="88"/>
+      <c r="J74" s="85"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" s="43" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="27"/>
       <c r="E75" s="27"/>
-      <c r="F75" s="88"/>
+      <c r="F75" s="85"/>
       <c r="G75" s="26"/>
       <c r="H75" s="27" t="s">
         <v>5</v>
@@ -4963,18 +5034,18 @@
       <c r="I75" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="J75" s="88"/>
+      <c r="J75" s="85"/>
     </row>
     <row r="76" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="47" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="19"/>
       <c r="E76" s="19"/>
-      <c r="F76" s="89"/>
+      <c r="F76" s="87"/>
       <c r="G76" s="18"/>
       <c r="H76" s="19" t="s">
         <v>5</v>
@@ -4982,15 +5053,20 @@
       <c r="I76" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="J76" s="89"/>
+      <c r="J76" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="J50:J56"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="F50:F56"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="B46:J47"/>
+    <mergeCell ref="J64:J76"/>
+    <mergeCell ref="F64:F76"/>
+    <mergeCell ref="G62:J62"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="B60:J61"/>
+    <mergeCell ref="B34:J35"/>
+    <mergeCell ref="J38:J42"/>
+    <mergeCell ref="F38:F42"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="C36:F36"/>
     <mergeCell ref="B4:J5"/>
     <mergeCell ref="B18:F19"/>
     <mergeCell ref="B20:B21"/>
@@ -5000,16 +5076,11 @@
     <mergeCell ref="J8:J14"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="F8:F14"/>
-    <mergeCell ref="B34:J35"/>
-    <mergeCell ref="J38:J42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="J64:J76"/>
-    <mergeCell ref="F64:F76"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="B60:J61"/>
+    <mergeCell ref="J50:J56"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="F50:F56"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="B46:J47"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5031,34 +5102,34 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="58"/>
+      <c r="B4" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="79"/>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="61"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="82"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
+      <c r="B6" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="77"/>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
@@ -5077,11 +5148,11 @@
         <v>4</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="72"/>
+      <c r="F8" s="62"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -5092,7 +5163,7 @@
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
-      <c r="F9" s="73"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -5105,7 +5176,7 @@
       <c r="E10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="73"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -5118,11 +5189,11 @@
       <c r="E11" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="73"/>
+      <c r="F11" s="63"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>5</v>
@@ -5131,11 +5202,11 @@
         <v>5</v>
       </c>
       <c r="E12" s="27"/>
-      <c r="F12" s="73"/>
+      <c r="F12" s="63"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>6</v>
@@ -5144,11 +5215,11 @@
         <v>5</v>
       </c>
       <c r="E13" s="27"/>
-      <c r="F13" s="73"/>
+      <c r="F13" s="63"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>5</v>
@@ -5157,11 +5228,11 @@
         <v>5</v>
       </c>
       <c r="E14" s="27"/>
-      <c r="F14" s="73"/>
+      <c r="F14" s="63"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>5</v>
@@ -5170,11 +5241,11 @@
         <v>5</v>
       </c>
       <c r="E15" s="27"/>
-      <c r="F15" s="73"/>
+      <c r="F15" s="63"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>5</v>
@@ -5183,11 +5254,11 @@
         <v>5</v>
       </c>
       <c r="E16" s="27"/>
-      <c r="F16" s="73"/>
+      <c r="F16" s="63"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>5</v>
@@ -5196,11 +5267,11 @@
         <v>5</v>
       </c>
       <c r="E17" s="27"/>
-      <c r="F17" s="73"/>
+      <c r="F17" s="63"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>5</v>
@@ -5209,24 +5280,24 @@
         <v>5</v>
       </c>
       <c r="E18" s="27"/>
-      <c r="F18" s="73"/>
+      <c r="F18" s="63"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="27"/>
-      <c r="F19" s="73"/>
+      <c r="F19" s="63"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>5</v>
@@ -5235,11 +5306,11 @@
         <v>5</v>
       </c>
       <c r="E20" s="27"/>
-      <c r="F20" s="73"/>
+      <c r="F20" s="63"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>5</v>
@@ -5248,11 +5319,11 @@
         <v>5</v>
       </c>
       <c r="E21" s="27"/>
-      <c r="F21" s="73"/>
+      <c r="F21" s="63"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>5</v>
@@ -5261,11 +5332,11 @@
         <v>5</v>
       </c>
       <c r="E22" s="27"/>
-      <c r="F22" s="73"/>
+      <c r="F22" s="63"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>5</v>
@@ -5274,11 +5345,11 @@
         <v>5</v>
       </c>
       <c r="E23" s="27"/>
-      <c r="F23" s="73"/>
+      <c r="F23" s="63"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>5</v>
@@ -5287,11 +5358,11 @@
         <v>5</v>
       </c>
       <c r="E24" s="27"/>
-      <c r="F24" s="73"/>
+      <c r="F24" s="63"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>5</v>
@@ -5300,11 +5371,11 @@
         <v>5</v>
       </c>
       <c r="E25" s="27"/>
-      <c r="F25" s="73"/>
+      <c r="F25" s="63"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>5</v>
@@ -5313,11 +5384,11 @@
         <v>5</v>
       </c>
       <c r="E26" s="27"/>
-      <c r="F26" s="73"/>
+      <c r="F26" s="63"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>5</v>
@@ -5326,7 +5397,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="19"/>
-      <c r="F27" s="74"/>
+      <c r="F27" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>